<commit_message>
Add report for covered pairs
</commit_message>
<xml_diff>
--- a/scripts/pairs.xlsx
+++ b/scripts/pairs.xlsx
@@ -466,12 +466,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>high_detail</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>n_ratings</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>high_detail</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -491,17 +491,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>splats/mcmc-truck-low-1.ksplat</t>
+          <t>splats/mcmc-truck-extended-1.ksplat</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>splats/default-truck-low-1.ksplat</t>
+          <t>splats/default-truck-extended-1.ksplat</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>low</t>
+          <t>extended</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -514,15 +514,15 @@
           <t>[0.58, 0.0, 0.65]</t>
         </is>
       </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="b">
-        <v>0</v>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>2</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>05bDTzubIAQcN7s6AkHs</t>
+          <t>5dwojHXzFd2RzJ2ZPNtD</t>
         </is>
       </c>
     </row>
@@ -537,17 +537,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>splats/mcmc-truck-extended-1.ksplat</t>
+          <t>splats/mcmc-truck-medium-1.ksplat</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>splats/default-truck-extended-1.ksplat</t>
+          <t>splats/default-truck-medium-1.ksplat</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>extended</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -560,15 +560,15 @@
           <t>[0.58, 0.0, 0.65]</t>
         </is>
       </c>
-      <c r="H3" t="n">
+      <c r="H3" t="b">
         <v>0</v>
       </c>
-      <c r="I3" t="b">
-        <v>1</v>
+      <c r="I3" t="n">
+        <v>2</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Lk507yRU9Gcvoqr66PTD</t>
+          <t>BGOjoywll3sSUYo2pBwY</t>
         </is>
       </c>
     </row>
@@ -583,17 +583,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>splats/mcmc-truck-medium-1.ksplat</t>
+          <t>splats/mcmc-truck-low-1.ksplat</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>splats/default-truck-medium-1.ksplat</t>
+          <t>splats/default-truck-low-1.ksplat</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>medium</t>
+          <t>low</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -606,15 +606,15 @@
           <t>[0.58, 0.0, 0.65]</t>
         </is>
       </c>
-      <c r="H4" t="n">
+      <c r="H4" t="b">
         <v>0</v>
       </c>
-      <c r="I4" t="b">
-        <v>0</v>
+      <c r="I4" t="n">
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>bzNWpl95kMDv3tzBcsHr</t>
+          <t>OyhrkDZsWy64SkqfZAY5</t>
         </is>
       </c>
     </row>
@@ -652,15 +652,15 @@
           <t>[0.58, 0.0, 0.65]</t>
         </is>
       </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="b">
+      <c r="H5" t="b">
         <v>1</v>
       </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>gLnu0rNhjibQDbl0lUjC</t>
+          <t>PqpflZDmB5tBiM15v9MQ</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add simple report for ratings per user
</commit_message>
<xml_diff>
--- a/scripts/pairs.xlsx
+++ b/scripts/pairs.xlsx
@@ -518,7 +518,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -564,7 +564,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -610,7 +610,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -656,7 +656,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Extend report for databse
</commit_message>
<xml_diff>
--- a/scripts/pairs.xlsx
+++ b/scripts/pairs.xlsx
@@ -518,7 +518,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -564,7 +564,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -610,7 +610,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -656,7 +656,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Redo report after Jan
</commit_message>
<xml_diff>
--- a/scripts/pairs.xlsx
+++ b/scripts/pairs.xlsx
@@ -732,7 +732,7 @@
         <v>1.793767186067828</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -792,7 +792,7 @@
         <v>1.500722891566265</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -852,7 +852,7 @@
         <v>1.500722891566265</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -1032,7 +1032,7 @@
         <v>1.500722891566265</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1572,7 +1572,7 @@
         <v>1.500722891566265</v>
       </c>
       <c r="M19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" t="inlineStr">
         <is>
@@ -1692,7 +1692,7 @@
         <v>1.508484848484849</v>
       </c>
       <c r="M21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21" t="inlineStr">
         <is>
@@ -1872,7 +1872,7 @@
         <v>1.508484848484849</v>
       </c>
       <c r="M24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" t="inlineStr">
         <is>
@@ -2052,7 +2052,7 @@
         <v>1.793767186067828</v>
       </c>
       <c r="M27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N27" t="inlineStr">
         <is>
@@ -2232,7 +2232,7 @@
         <v>1.508484848484849</v>
       </c>
       <c r="M30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N30" t="inlineStr">
         <is>
@@ -2292,7 +2292,7 @@
         <v>1.508484848484849</v>
       </c>
       <c r="M31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N31" t="inlineStr">
         <is>
@@ -3372,7 +3372,7 @@
         <v>1.793767186067828</v>
       </c>
       <c r="M49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N49" t="inlineStr">
         <is>

</xml_diff>